<commit_message>
Changes from 5/28 - 6/4
- Generate Trajectories from a predefined path.
- Upgraded most slammer things to the servos
- Added a class to do all the math for the follower wheel
- Added a class to follow a Path
- Added a class to store paths, so we don't have to recalculate them every time we init the robot
- Added automation code for the slammer and stopped to make sure they don't collide
- Removed Relic from the Robot till we get it on the robot
- Removed Relic code from teleop
- Removed the AutoTransitioner for now bc it takes time
- Moved files around
</commit_message>
<xml_diff>
--- a/Finding_kV_andkA.xlsx
+++ b/Finding_kV_andkA.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Calculated" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Real Max Value</t>
   </si>
@@ -87,6 +87,9 @@
   <si>
     <t>Acc (In/Sec^2)</t>
   </si>
+  <si>
+    <t>Hz</t>
+  </si>
 </sst>
 </file>
 
@@ -94,7 +97,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000000000"/>
-    <numFmt numFmtId="170" formatCode="0.0000000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000000"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -637,7 +640,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -652,12 +655,15 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -5934,14 +5940,14 @@
   <dimension ref="A1:G168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.42578125" customWidth="1"/>
+    <col min="4" max="4" width="0.140625" customWidth="1"/>
     <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -5973,6 +5979,10 @@
       <c r="C2" s="5">
         <v>46400314.2827117</v>
       </c>
+      <c r="D2">
+        <f>IF(A2&lt;1,1,"")</f>
+        <v>1</v>
+      </c>
       <c r="E2" s="7" t="s">
         <v>0</v>
       </c>
@@ -5995,6 +6005,10 @@
       <c r="C3" s="5">
         <v>139453098.09140801</v>
       </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D66" si="0">IF(A3&lt;1,1,"")</f>
+        <v>1</v>
+      </c>
       <c r="E3" s="7" t="s">
         <v>1</v>
       </c>
@@ -6017,6 +6031,10 @@
       <c r="C4" s="5">
         <v>54335982.460800998</v>
       </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="E4" s="7" t="s">
         <v>4</v>
       </c>
@@ -6039,6 +6057,10 @@
       <c r="C5" s="4">
         <v>445260.56651464698</v>
       </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="E5" s="7" t="s">
         <v>5</v>
       </c>
@@ -6061,6 +6083,10 @@
       <c r="C6" s="5">
         <v>35065137.325867899</v>
       </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -6073,6 +6099,10 @@
       <c r="C7" s="5">
         <v>138995336.77598399</v>
       </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="E7" s="3" t="s">
         <v>6</v>
       </c>
@@ -6090,6 +6120,10 @@
       </c>
       <c r="C8" s="4">
         <v>6484036.0817845399</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="2">
@@ -6111,6 +6145,10 @@
       <c r="C9" s="4">
         <v>6678868.6042649904</v>
       </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="E9" s="3" t="s">
         <v>7</v>
       </c>
@@ -6133,6 +6171,10 @@
       <c r="C10" s="5">
         <v>22992773.6901136</v>
       </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -6144,6 +6186,10 @@
       <c r="C11" s="5">
         <v>223942666.29755199</v>
       </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -6155,6 +6201,17 @@
       <c r="C12" s="5">
         <v>42268351.393012501</v>
       </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="6">
+        <f>SUM(D:D)</f>
+        <v>146</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -6166,6 +6223,10 @@
       <c r="C13" s="5">
         <v>150799962.038378</v>
       </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -6177,6 +6238,10 @@
       <c r="C14" s="5">
         <v>130033158.75376099</v>
       </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -6188,6 +6253,10 @@
       <c r="C15" s="5">
         <v>65921420.312395804</v>
       </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -6199,8 +6268,12 @@
       <c r="C16" s="5">
         <v>133077045.492979</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0.15688333400000001</v>
       </c>
@@ -6210,8 +6283,12 @@
       <c r="C17" s="5">
         <v>63985048.700894803</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0.16286005200000001</v>
       </c>
@@ -6221,8 +6298,12 @@
       <c r="C18" s="5">
         <v>206392696.363792</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0.170035677</v>
       </c>
@@ -6232,8 +6313,12 @@
       <c r="C19" s="5">
         <v>87729537.663836598</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0.177900365</v>
       </c>
@@ -6243,8 +6328,12 @@
       <c r="C20" s="5">
         <v>111745884.32041</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0.18500593800000001</v>
       </c>
@@ -6254,8 +6343,12 @@
       <c r="C21" s="5">
         <v>96218675.348635405</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0.19691375</v>
       </c>
@@ -6265,8 +6358,12 @@
       <c r="C22" s="5">
         <v>88739521.597453207</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0.200909844</v>
       </c>
@@ -6276,8 +6373,12 @@
       <c r="C23" s="5">
         <v>39858170.302805297</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0.20592885499999999</v>
       </c>
@@ -6287,8 +6388,12 @@
       <c r="C24" s="5">
         <v>94246111.649658903</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0.21198541700000001</v>
       </c>
@@ -6298,8 +6403,12 @@
       <c r="C25" s="5">
         <v>12080566.4009673</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0.21796281300000001</v>
       </c>
@@ -6309,8 +6418,12 @@
       <c r="C26" s="5">
         <v>79322145.821945295</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0.22688958400000001</v>
       </c>
@@ -6320,8 +6433,12 @@
       <c r="C27" s="5">
         <v>438686408.12166399</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0.23387187500000001</v>
       </c>
@@ -6331,8 +6448,12 @@
       <c r="C28" s="5">
         <v>167074717.13709199</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>0.23987729199999999</v>
       </c>
@@ -6342,8 +6463,12 @@
       <c r="C29" s="5">
         <v>63457716.657556199</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0.246864584</v>
       </c>
@@ -6353,8 +6478,12 @@
       <c r="C30" s="5">
         <v>494659500.14834899</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0.25387151000000002</v>
       </c>
@@ -6364,8 +6493,12 @@
       <c r="C31" s="5">
         <v>147660640.408968</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>0.25987322899999998</v>
       </c>
@@ -6375,8 +6508,12 @@
       <c r="C32" s="5">
         <v>116194755.57023101</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>0.26596739600000002</v>
       </c>
@@ -6386,8 +6523,12 @@
       <c r="C33" s="5">
         <v>123407230.629085</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>0.27195328099999999</v>
       </c>
@@ -6397,8 +6538,12 @@
       <c r="C34" s="5">
         <v>44669917.273782998</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>0.27591046899999999</v>
       </c>
@@ -6408,8 +6553,12 @@
       <c r="C35" s="4">
         <v>684510.71883152798</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>0.28296843700000002</v>
       </c>
@@ -6419,8 +6568,12 @@
       <c r="C36" s="5">
         <v>444797321.44002002</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>0.28992734399999998</v>
       </c>
@@ -6430,8 +6583,12 @@
       <c r="C37" s="5">
         <v>494487112.34372699</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>0.29393437500000003</v>
       </c>
@@ -6441,8 +6598,12 @@
       <c r="C38" s="4">
         <v>437881.958089869</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>0.29687593699999998</v>
       </c>
@@ -6452,8 +6613,12 @@
       <c r="C39" s="5">
         <v>58492862.500272103</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>0.30295343600000002</v>
       </c>
@@ -6463,8 +6628,12 @@
       <c r="C40" s="5">
         <v>103624029.434572</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>0.309847551</v>
       </c>
@@ -6474,8 +6643,12 @@
       <c r="C41" s="5">
         <v>475238360.57483298</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>0.31601791600000001</v>
       </c>
@@ -6485,8 +6658,12 @@
       <c r="C42" s="4">
         <v>7453539.8785255197</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>0.32197218599999999</v>
       </c>
@@ -6496,8 +6673,12 @@
       <c r="C43" s="5">
         <v>26062706.599147201</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>0.33085812399999998</v>
       </c>
@@ -6507,8 +6688,12 @@
       <c r="C44" s="4">
         <v>2120310.20903312</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>0.33895124799999998</v>
       </c>
@@ -6518,8 +6703,12 @@
       <c r="C45" s="5">
         <v>373121708.84662998</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>0.34497140399999998</v>
       </c>
@@ -6529,8 +6718,12 @@
       <c r="C46" s="4">
         <v>932759.54499171895</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>0.347930727</v>
       </c>
@@ -6540,8 +6733,12 @@
       <c r="C47" s="5">
         <v>45641321.997627601</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>0.353908956</v>
       </c>
@@ -6551,8 +6748,12 @@
       <c r="C48" s="5">
         <v>27058038.586789701</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>0.360840259</v>
       </c>
@@ -6562,8 +6763,12 @@
       <c r="C49" s="5">
         <v>552281917.95176303</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>0.36801213399999999</v>
       </c>
@@ -6573,8 +6778,12 @@
       <c r="C50" s="4">
         <v>3845131.79324377</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>0.37590619800000002</v>
       </c>
@@ -6584,8 +6793,12 @@
       <c r="C51" s="4">
         <v>1828272.9203069501</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>0.38188296799999999</v>
       </c>
@@ -6595,8 +6808,12 @@
       <c r="C52" s="5">
         <v>187603509.49765399</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>0.38987968699999997</v>
       </c>
@@ -6606,8 +6823,12 @@
       <c r="C53" s="5">
         <v>163341269.30543599</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>0.39588161399999999</v>
       </c>
@@ -6617,8 +6838,12 @@
       <c r="C54" s="5">
         <v>584955177.70355904</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>0.40188359299999998</v>
       </c>
@@ -6628,8 +6853,12 @@
       <c r="C55" s="5">
         <v>127615447.037304</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>0.40793291599999998</v>
       </c>
@@ -6639,8 +6868,12 @@
       <c r="C56" s="5">
         <v>631723961.19701397</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>0.41390895700000002</v>
       </c>
@@ -6650,8 +6883,12 @@
       <c r="C57" s="5">
         <v>144119202.57812199</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>0.41985609299999999</v>
       </c>
@@ -6661,8 +6898,12 @@
       <c r="C58" s="5">
         <v>642551927.15909195</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>0.426506145</v>
       </c>
@@ -6672,8 +6913,12 @@
       <c r="C59" s="4">
         <v>136746.06830041</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>0.432902499</v>
       </c>
@@ -6683,8 +6928,12 @@
       <c r="C60" s="5">
         <v>798824749.94553995</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>0.44320208300000002</v>
       </c>
@@ -6694,8 +6943,12 @@
       <c r="C61" s="5">
         <v>189025548.07155201</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>0.449193385</v>
       </c>
@@ -6705,8 +6958,12 @@
       <c r="C62" s="5">
         <v>212308509.66240999</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>0.45512088499999998</v>
       </c>
@@ -6716,8 +6973,12 @@
       <c r="C63" s="5">
         <v>135883352.71605101</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>0.46198072800000001</v>
       </c>
@@ -6727,8 +6988,12 @@
       <c r="C64" s="5">
         <v>359327514.47901201</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>0.46810145800000003</v>
       </c>
@@ -6738,8 +7003,12 @@
       <c r="C65" s="5">
         <v>224360980.850234</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>0.47701427000000002</v>
       </c>
@@ -6749,8 +7018,12 @@
       <c r="C66" s="5">
         <v>92241148.131259695</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>0.480948072</v>
       </c>
@@ -6760,8 +7033,12 @@
       <c r="C67" s="5">
         <v>428367951.43939</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67">
+        <f t="shared" ref="D67:D130" si="1">IF(A67&lt;1,1,"")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>0.487954479</v>
       </c>
@@ -6771,8 +7048,12 @@
       <c r="C68" s="5">
         <v>785907154.04353797</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>0.49094354099999998</v>
       </c>
@@ -6782,8 +7063,12 @@
       <c r="C69" s="5">
         <v>195078104.76011699</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>0.49794598899999998</v>
       </c>
@@ -6793,8 +7078,12 @@
       <c r="C70" s="5">
         <v>649053994.39293897</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>0.50492906199999998</v>
       </c>
@@ -6804,8 +7093,12 @@
       <c r="C71" s="5">
         <v>385588025.87260801</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>0.51197567600000005</v>
       </c>
@@ -6815,8 +7108,12 @@
       <c r="C72" s="4">
         <v>8340797.9951154198</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>0.51533619799999997</v>
       </c>
@@ -6826,8 +7123,12 @@
       <c r="C73" s="4">
         <v>230102.88672939999</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>0.52110682200000003</v>
       </c>
@@ -6837,8 +7138,12 @@
       <c r="C74" s="5">
         <v>275946302.774602</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>0.52899666599999995</v>
       </c>
@@ -6848,8 +7153,12 @@
       <c r="C75" s="5">
         <v>750637748.31013095</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>0.53599426999999999</v>
       </c>
@@ -6859,8 +7168,12 @@
       <c r="C76" s="5">
         <v>415358131.80415601</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>0.54291760300000003</v>
       </c>
@@ -6870,8 +7183,12 @@
       <c r="C77" s="5">
         <v>211105959.171388</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>0.54908265599999995</v>
       </c>
@@ -6881,8 +7198,12 @@
       <c r="C78" s="5">
         <v>821123109.75768602</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>0.55501572899999996</v>
       </c>
@@ -6892,8 +7213,12 @@
       <c r="C79" s="5">
         <v>119922659.537936</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>0.56091713499999996</v>
       </c>
@@ -6903,8 +7228,12 @@
       <c r="C80" s="5">
         <v>706700625.195189</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>0.566846666</v>
       </c>
@@ -6914,8 +7243,12 @@
       <c r="C81" s="5">
         <v>218947894.59985501</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>0.57009531199999997</v>
       </c>
@@ -6925,8 +7258,12 @@
       <c r="C82" s="5">
         <v>378465549.48635799</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>0.57787614499999995</v>
       </c>
@@ -6936,8 +7273,12 @@
       <c r="C83" s="5">
         <v>788425648.53694403</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>0.58306161400000001</v>
       </c>
@@ -6947,8 +7288,12 @@
       <c r="C84" s="5">
         <v>279646717.47034401</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>0.58892177000000001</v>
       </c>
@@ -6958,8 +7303,12 @@
       <c r="C85" s="4">
         <v>2101317.1469387198</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>0.59194291600000004</v>
       </c>
@@ -6969,8 +7318,12 @@
       <c r="C86" s="5">
         <v>66823354.6820032</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>0.59898020799999996</v>
       </c>
@@ -6980,8 +7333,12 @@
       <c r="C87" s="5">
         <v>801663074.98804903</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>0.60508307299999997</v>
       </c>
@@ -6991,8 +7348,12 @@
       <c r="C88" s="5">
         <v>245084054.50097099</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>0.61397906199999996</v>
       </c>
@@ -7002,8 +7363,12 @@
       <c r="C89" s="5">
         <v>1169910355.40711</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>0.61789359300000002</v>
       </c>
@@ -7013,8 +7378,12 @@
       <c r="C90" s="5">
         <v>113689173.55287801</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D90">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>0.624237916</v>
       </c>
@@ -7024,8 +7393,12 @@
       <c r="C91" s="5">
         <v>459621874.47340697</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D91">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>0.63189223900000002</v>
       </c>
@@ -7035,8 +7408,12 @@
       <c r="C92" s="5">
         <v>379021723.99994701</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D92">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>0.63893270800000002</v>
       </c>
@@ -7046,8 +7423,12 @@
       <c r="C93" s="5">
         <v>744258330.49842894</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D93">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>0.64404697799999999</v>
       </c>
@@ -7057,8 +7438,12 @@
       <c r="C94" s="5">
         <v>234961257.853221</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D94">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>0.64995442599999997</v>
       </c>
@@ -7068,8 +7453,12 @@
       <c r="C95" s="5">
         <v>731144013.53610802</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D95">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>0.65693005199999999</v>
       </c>
@@ -7079,8 +7468,12 @@
       <c r="C96" s="5">
         <v>947295237.96617806</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D96">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>0.66293192599999995</v>
       </c>
@@ -7090,8 +7483,12 @@
       <c r="C97" s="5">
         <v>728784613.62550497</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D97">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>0.66895406199999996</v>
       </c>
@@ -7101,8 +7498,12 @@
       <c r="C98" s="5">
         <v>806926108.80910206</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D98">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>0.67495348899999996</v>
       </c>
@@ -7112,8 +7513,12 @@
       <c r="C99" s="5">
         <v>15165147.458459301</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D99">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>0.68094828100000004</v>
       </c>
@@ -7123,8 +7528,12 @@
       <c r="C100" s="5">
         <v>255419592.504899</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D100">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>0.68844775999999996</v>
       </c>
@@ -7134,8 +7543,12 @@
       <c r="C101" s="5">
         <v>18033201.7618002</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D101">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>0.69501260399999998</v>
       </c>
@@ -7145,8 +7558,12 @@
       <c r="C102" s="5">
         <v>934453623.13309598</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D102">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>0.70297385300000004</v>
       </c>
@@ -7156,8 +7573,12 @@
       <c r="C103" s="5">
         <v>960403523.42379105</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D103">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>0.71097270800000001</v>
       </c>
@@ -7167,8 +7588,12 @@
       <c r="C104" s="5">
         <v>1189119749.0632601</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D104">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>0.71819317699999996</v>
       </c>
@@ -7178,8 +7603,12 @@
       <c r="C105" s="4">
         <v>4529106.4060256202</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D105">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>0.72399932199999995</v>
       </c>
@@ -7189,8 +7618,12 @@
       <c r="C106" s="5">
         <v>895555460.02194202</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D106">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>0.73100619700000002</v>
       </c>
@@ -7200,8 +7633,12 @@
       <c r="C107" s="5">
         <v>963661212.17524397</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D107">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>0.73906744700000004</v>
       </c>
@@ -7211,8 +7648,12 @@
       <c r="C108" s="5">
         <v>473234639.23533899</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D108">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>0.74492828099999997</v>
       </c>
@@ -7222,8 +7663,12 @@
       <c r="C109" s="5">
         <v>462227051.232333</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D109">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>0.75288953000000003</v>
       </c>
@@ -7233,8 +7678,12 @@
       <c r="C110" s="5">
         <v>907872284.84453499</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D110">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>0.75889796799999998</v>
       </c>
@@ -7244,8 +7693,12 @@
       <c r="C111" s="5">
         <v>162591101.673163</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D111">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>0.76602650999999999</v>
       </c>
@@ -7255,8 +7708,12 @@
       <c r="C112" s="5">
         <v>18749050.671889</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D112">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>0.77086255100000001</v>
       </c>
@@ -7266,8 +7723,12 @@
       <c r="C113" s="5">
         <v>284408605.80989802</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D113">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>0.77787150999999999</v>
       </c>
@@ -7277,8 +7738,12 @@
       <c r="C114" s="5">
         <v>12610242.1074252</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D114">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>0.78393223899999998</v>
       </c>
@@ -7288,8 +7753,12 @@
       <c r="C115" s="4">
         <v>6920962.3667702395</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D115">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>0.78984963500000005</v>
       </c>
@@ -7299,8 +7768,12 @@
       <c r="C116" s="4">
         <v>773018.63686067599</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D116">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>0.79697203100000003</v>
       </c>
@@ -7310,8 +7783,12 @@
       <c r="C117" s="4">
         <v>2296606.82996898</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D117">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>0.80297874899999999</v>
       </c>
@@ -7321,8 +7798,12 @@
       <c r="C118" s="5">
         <v>399419211.31090498</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D118">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>0.80896583300000002</v>
       </c>
@@ -7332,8 +7813,12 @@
       <c r="C119" s="4">
         <v>1703663.65917604</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D119">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>0.81499218699999998</v>
       </c>
@@ -7343,8 +7828,12 @@
       <c r="C120" s="4">
         <v>1589610.9931515399</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D120">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>0.82186854099999995</v>
       </c>
@@ -7354,8 +7843,12 @@
       <c r="C121" s="5">
         <v>473947595.53992897</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D121">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>0.82886124900000002</v>
       </c>
@@ -7365,8 +7858,12 @@
       <c r="C122" s="4">
         <v>6749085.4628918702</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D122">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>0.83580510399999997</v>
       </c>
@@ -7376,8 +7873,12 @@
       <c r="C123" s="5">
         <v>836087724.58284104</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D123">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>0.84385942599999997</v>
       </c>
@@ -7387,8 +7888,12 @@
       <c r="C124" s="4">
         <v>9194281.2770206705</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D124">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>0.851917916</v>
       </c>
@@ -7398,8 +7903,12 @@
       <c r="C125" s="4">
         <v>4019472.8384725298</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D125">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>0.85787499899999997</v>
       </c>
@@ -7409,8 +7918,12 @@
       <c r="C126" s="5">
         <v>564282988.23909402</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D126">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>0.863866562</v>
       </c>
@@ -7420,8 +7933,12 @@
       <c r="C127" s="4">
         <v>6571821.3675309401</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D127">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>0.872965624</v>
       </c>
@@ -7431,8 +7948,12 @@
       <c r="C128" s="4">
         <v>2497757.5629439699</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D128">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>0.87896916599999997</v>
       </c>
@@ -7442,8 +7963,12 @@
       <c r="C129" s="4">
         <v>2168290.12775992</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D129">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>0.88185338499999999</v>
       </c>
@@ -7453,8 +7978,12 @@
       <c r="C130" s="4">
         <v>3483833.19457694</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D130">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>0.88793395799999997</v>
       </c>
@@ -7464,8 +7993,12 @@
       <c r="C131" s="4">
         <v>2447180.8042880301</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D131">
+        <f t="shared" ref="D131:D153" si="2">IF(A131&lt;1,1,"")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>0.89706098899999998</v>
       </c>
@@ -7475,8 +8008,12 @@
       <c r="C132" s="5">
         <v>679093079.76626396</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D132">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>0.90532708299999998</v>
       </c>
@@ -7486,8 +8023,12 @@
       <c r="C133" s="5">
         <v>121017143.45578</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D133">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>0.91285838500000005</v>
       </c>
@@ -7497,8 +8038,12 @@
       <c r="C134" s="5">
         <v>588504318.43911302</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D134">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>0.91885786400000002</v>
       </c>
@@ -7508,8 +8053,12 @@
       <c r="C135" s="4">
         <v>3657417.5557972598</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D135">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>0.92497807300000001</v>
       </c>
@@ -7519,8 +8068,12 @@
       <c r="C136" s="5">
         <v>19815464.201104801</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D136">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>0.93230833199999996</v>
       </c>
@@ -7530,8 +8083,12 @@
       <c r="C137" s="5">
         <v>190384813.86947399</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D137">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>0.93686041600000003</v>
       </c>
@@ -7541,8 +8098,12 @@
       <c r="C138" s="4">
         <v>3221396.8438470801</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D138">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>0.94390140499999997</v>
       </c>
@@ -7552,8 +8113,12 @@
       <c r="C139" s="5">
         <v>457530548.84937501</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D139">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>0.947167447</v>
       </c>
@@ -7563,8 +8128,12 @@
       <c r="C140" s="4">
         <v>381682.34841839399</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D140">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>0.95296150999999996</v>
       </c>
@@ -7574,8 +8143,12 @@
       <c r="C141" s="4">
         <v>1533012.15879736</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D141">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>0.96011661400000003</v>
       </c>
@@ -7585,8 +8158,12 @@
       <c r="C142" s="4">
         <v>1010845.55827273</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D142">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>0.96819801999999999</v>
       </c>
@@ -7596,8 +8173,12 @@
       <c r="C143" s="4">
         <v>805974.42419398401</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D143">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>0.97506520799999996</v>
       </c>
@@ -7607,8 +8188,12 @@
       <c r="C144" s="4">
         <v>1111983.1636576001</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D144">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>0.981917135</v>
       </c>
@@ -7618,8 +8203,12 @@
       <c r="C145" s="5">
         <v>194426141.60071799</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D145">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>0.98497078100000002</v>
       </c>
@@ -7629,8 +8218,12 @@
       <c r="C146" s="4">
         <v>1048068.93191592</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D146">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>0.99300401000000005</v>
       </c>
@@ -7640,8 +8233,12 @@
       <c r="C147" s="5">
         <v>943004067.38327098</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D147">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>1.000021354</v>
       </c>
@@ -7651,8 +8248,12 @@
       <c r="C148" s="5">
         <v>170926834.98590899</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D148" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>1.00697802</v>
       </c>
@@ -7662,8 +8263,12 @@
       <c r="C149" s="5">
         <v>653196730.604738</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D149" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>1.014051509</v>
       </c>
@@ -7673,8 +8278,12 @@
       <c r="C150" s="5">
         <v>737013241.51097798</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D150" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>1.0219208849999999</v>
       </c>
@@ -7684,8 +8293,12 @@
       <c r="C151" s="4">
         <v>2618845.19160792</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D151" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>1.025194843</v>
       </c>
@@ -7695,8 +8308,12 @@
       <c r="C152" s="5">
         <v>374361453.853607</v>
       </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D152" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>1.0310801549999999</v>
       </c>
@@ -7706,8 +8323,12 @@
       <c r="C153" s="5">
         <v>343302232.23119098</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D153" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>1.036857916</v>
       </c>
@@ -7718,7 +8339,7 @@
         <v>3430487.28529872</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>1.0400538530000001</v>
       </c>
@@ -7729,7 +8350,7 @@
         <v>6910970.0443527596</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>1.046891145</v>
       </c>
@@ -7740,7 +8361,7 @@
         <v>34384256.647875801</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>1.0539055719999999</v>
       </c>
@@ -7751,7 +8372,7 @@
         <v>31314852.987199198</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>1.0609130200000001</v>
       </c>
@@ -7762,7 +8383,7 @@
         <v>560513812.68574595</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>1.0669169789999999</v>
       </c>
@@ -7773,7 +8394,7 @@
         <v>463327152.68285698</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>1.073068801</v>
       </c>

</xml_diff>